<commit_message>
Atualizando dicionário de dados utilizado
</commit_message>
<xml_diff>
--- a/docs/dicionario de dados.xlsx
+++ b/docs/dicionario de dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE0E34E-F686-412C-A59C-5EF751FB64F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9025DEB-7EB9-42F4-B7FD-270E703FA54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B89CA311-6F3B-435C-810C-AE3ADE056328}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>data_nascimento</t>
   </si>
@@ -80,9 +80,6 @@
     <t>forma_ingresso</t>
   </si>
   <si>
-    <t>historico_disciplinas</t>
-  </si>
-  <si>
     <t>frequencia</t>
   </si>
   <si>
@@ -288,6 +285,21 @@
   </si>
   <si>
     <t>Modalidade que o aluno está matriculado (Presencial, EAD ou Hibrido)</t>
+  </si>
+  <si>
+    <t>disciplinas_cursadas</t>
+  </si>
+  <si>
+    <t>data_evasao</t>
+  </si>
+  <si>
+    <t>Data de evasão do aluno</t>
+  </si>
+  <si>
+    <t>semestre</t>
+  </si>
+  <si>
+    <t>Semestre que o aluno está estudando. Caso ele tiver evadido, é o semestre que ele evadiu.</t>
   </si>
 </sst>
 </file>
@@ -407,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -418,16 +430,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -440,13 +446,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,17 +787,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3BB862-F8C2-4766-9C90-DEF98465B36A}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="69.85546875" customWidth="1"/>
+    <col min="3" max="3" width="80" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
@@ -800,554 +806,585 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
+      <c r="B20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" ht="17.25" customHeight="1">
+      <c r="A21" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
+        <v>83</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
+        <v>14</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
+        <v>16</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
+        <v>28</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
+        <v>18</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
+        <v>22</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
+        <v>24</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>